<commit_message>
had to strip in parse.py
</commit_message>
<xml_diff>
--- a/data/ForPrincetonCompSciTeam_10-7.xlsx
+++ b/data/ForPrincetonCompSciTeam_10-7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinabeshai/School/Junior/Fall/COS333i/fair-share-housing-5/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB5CC02-DDED-B14A-8A98-E6C21FD6903E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB709AD1-12F5-8D4F-938E-9D3D71236777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27480" windowHeight="16140" xr2:uid="{129652EC-9F8C-3B42-82FF-3C73F84312CD}"/>
   </bookViews>
@@ -2035,10 +2035,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CD3CD4-8082-984A-BCC5-8BEEC687BD02}">
   <dimension ref="A1:AY159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="W1" sqref="W1"/>
-      <selection pane="bottomLeft" activeCell="AM1" sqref="AM1"/>
+      <selection pane="bottomLeft" activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2048,7 +2048,9 @@
     <col min="6" max="6" width="21.6640625" style="3" customWidth="1"/>
     <col min="7" max="10" width="10.83203125" style="3"/>
     <col min="11" max="11" width="93" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="3"/>
+    <col min="12" max="25" width="10.83203125" style="3"/>
+    <col min="26" max="26" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="68" x14ac:dyDescent="0.2">

</xml_diff>